<commit_message>
Atualizações dos templates 01 ao 14
</commit_message>
<xml_diff>
--- a/23. Matrizes_de_Reastriabilidade(caracteristicas_X_SSS).xlsx
+++ b/23. Matrizes_de_Reastriabilidade(caracteristicas_X_SSS).xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Elton\Desktop\OPE\OPE_Artefatos_HAIR2U\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{93A33058-7EE2-4561-BD6E-ADA27D2B60DA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C0190506-5805-491A-BD88-B2DC669D652D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{89EBB04A-67B7-4AA4-AAF3-D9E552B7152C}"/>
+    <workbookView xWindow="-39975" yWindow="4335" windowWidth="17280" windowHeight="8400" xr2:uid="{89EBB04A-67B7-4AA4-AAF3-D9E552B7152C}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="47">
   <si>
     <t>ID</t>
   </si>
@@ -197,12 +197,6 @@
     <t>Listas de serviços</t>
   </si>
   <si>
-    <t>Funcionalidades</t>
-  </si>
-  <si>
-    <t>Comunicação</t>
-  </si>
-  <si>
     <t>Divulgação e parceria</t>
   </si>
   <si>
@@ -239,13 +233,16 @@
     <t>X</t>
   </si>
   <si>
-    <t>Cadastro Clientes</t>
-  </si>
-  <si>
     <t>O Sistema DEVE permitir que o cliente realize o pedido de encaixe no agendamento.</t>
   </si>
   <si>
     <t>SSS-0009:</t>
+  </si>
+  <si>
+    <t>Divulgação em vídeo</t>
+  </si>
+  <si>
+    <t>Comunicação com cliente</t>
   </si>
 </sst>
 </file>
@@ -400,24 +397,6 @@
     <xf numFmtId="0" fontId="5" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -428,6 +407,24 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -744,313 +741,305 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4AE06A75-DEF9-416D-A0BA-146A63DAFD2F}">
-  <dimension ref="A1:AI15"/>
+  <dimension ref="A1:AH15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="AI17" sqref="AI17"/>
+    <sheetView tabSelected="1" topLeftCell="Y1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="AK8" sqref="AK8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13" customWidth="1"/>
     <col min="9" max="9" width="9.140625" customWidth="1"/>
-    <col min="10" max="35" width="7" customWidth="1"/>
+    <col min="10" max="34" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13"/>
-      <c r="B1" s="13"/>
-      <c r="C1" s="13"/>
-      <c r="D1" s="13"/>
-      <c r="E1" s="13"/>
-      <c r="F1" s="13"/>
-      <c r="G1" s="13"/>
-      <c r="H1" s="13"/>
-      <c r="I1" s="13"/>
-      <c r="J1" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="K1" s="8"/>
-      <c r="L1" s="8"/>
-      <c r="M1" s="8"/>
-      <c r="N1" s="8"/>
-      <c r="O1" s="8"/>
-      <c r="P1" s="8"/>
-      <c r="Q1" s="8"/>
-      <c r="R1" s="8"/>
-      <c r="S1" s="8"/>
-      <c r="T1" s="8"/>
-      <c r="U1" s="8"/>
-      <c r="V1" s="8"/>
-      <c r="W1" s="8"/>
-      <c r="X1" s="8"/>
-      <c r="Y1" s="8"/>
-      <c r="Z1" s="8"/>
-      <c r="AA1" s="8"/>
-      <c r="AB1" s="8"/>
-      <c r="AC1" s="8"/>
-      <c r="AD1" s="8"/>
-      <c r="AE1" s="8"/>
-      <c r="AF1" s="8"/>
-      <c r="AG1" s="8"/>
-      <c r="AH1" s="8"/>
-      <c r="AI1" s="8"/>
+    <row r="1" spans="1:34" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="7"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
+      <c r="D1" s="7"/>
+      <c r="E1" s="7"/>
+      <c r="F1" s="7"/>
+      <c r="G1" s="7"/>
+      <c r="H1" s="7"/>
+      <c r="I1" s="7"/>
+      <c r="J1" s="13" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" s="14"/>
+      <c r="L1" s="14"/>
+      <c r="M1" s="14"/>
+      <c r="N1" s="14"/>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
+      <c r="T1" s="14"/>
+      <c r="U1" s="14"/>
+      <c r="V1" s="14"/>
+      <c r="W1" s="14"/>
+      <c r="X1" s="14"/>
+      <c r="Y1" s="14"/>
+      <c r="Z1" s="14"/>
+      <c r="AA1" s="14"/>
+      <c r="AB1" s="14"/>
+      <c r="AC1" s="14"/>
+      <c r="AD1" s="14"/>
+      <c r="AE1" s="14"/>
+      <c r="AF1" s="14"/>
+      <c r="AG1" s="14"/>
+      <c r="AH1" s="14"/>
     </row>
-    <row r="2" spans="1:35" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="13"/>
-      <c r="D2" s="13"/>
-      <c r="E2" s="13"/>
-      <c r="F2" s="13"/>
-      <c r="G2" s="13"/>
-      <c r="H2" s="13"/>
-      <c r="I2" s="13"/>
-      <c r="J2" s="9" t="s">
+    <row r="2" spans="1:34" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="7"/>
+      <c r="B2" s="7"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
+      <c r="I2" s="7"/>
+      <c r="J2" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="K2" s="10" t="s">
+      <c r="K2" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="L2" s="6" t="s">
+      <c r="L2" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="M2" s="5" t="s">
+      <c r="M2" s="12" t="s">
         <v>21</v>
       </c>
-      <c r="N2" s="6" t="s">
+      <c r="N2" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="O2" s="5" t="s">
+      <c r="O2" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="6" t="s">
+      <c r="P2" s="9" t="s">
         <v>24</v>
       </c>
-      <c r="Q2" s="5" t="s">
+      <c r="Q2" s="12" t="s">
         <v>25</v>
       </c>
-      <c r="R2" s="6" t="s">
+      <c r="R2" s="9" t="s">
         <v>26</v>
       </c>
-      <c r="S2" s="5" t="s">
+      <c r="S2" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="T2" s="6" t="s">
+      <c r="T2" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="U2" s="5" t="s">
+      <c r="U2" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="V2" s="6" t="s">
+      <c r="V2" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="W2" s="5" t="s">
+      <c r="W2" s="12" t="s">
+        <v>45</v>
+      </c>
+      <c r="X2" s="9" t="s">
+        <v>46</v>
+      </c>
+      <c r="Y2" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="X2" s="6" t="s">
+      <c r="Z2" s="9" t="s">
         <v>32</v>
       </c>
-      <c r="Y2" s="5" t="s">
+      <c r="AA2" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="Z2" s="6" t="s">
+      <c r="AB2" s="9" t="s">
         <v>34</v>
       </c>
-      <c r="AA2" s="5" t="s">
+      <c r="AC2" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="AB2" s="6" t="s">
+      <c r="AD2" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="AC2" s="5" t="s">
+      <c r="AE2" s="12" t="s">
         <v>37</v>
       </c>
-      <c r="AD2" s="6" t="s">
+      <c r="AF2" s="9" t="s">
         <v>38</v>
       </c>
-      <c r="AE2" s="5" t="s">
+      <c r="AG2" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="AF2" s="6" t="s">
+      <c r="AH2" s="9" t="s">
         <v>40</v>
       </c>
-      <c r="AG2" s="5" t="s">
-        <v>41</v>
-      </c>
-      <c r="AH2" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="AI2" s="6" t="s">
-        <v>45</v>
-      </c>
     </row>
-    <row r="3" spans="1:35" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13"/>
-      <c r="B3" s="13"/>
-      <c r="C3" s="13"/>
-      <c r="D3" s="13"/>
-      <c r="E3" s="13"/>
-      <c r="F3" s="13"/>
-      <c r="G3" s="13"/>
-      <c r="H3" s="13"/>
-      <c r="I3" s="13"/>
-      <c r="J3" s="9"/>
-      <c r="K3" s="10"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="6"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="6"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="6"/>
-      <c r="U3" s="5"/>
-      <c r="V3" s="6"/>
-      <c r="W3" s="5"/>
-      <c r="X3" s="6"/>
-      <c r="Y3" s="5"/>
-      <c r="Z3" s="6"/>
-      <c r="AA3" s="5"/>
-      <c r="AB3" s="6"/>
-      <c r="AC3" s="5"/>
-      <c r="AD3" s="6"/>
-      <c r="AE3" s="5"/>
-      <c r="AF3" s="6"/>
-      <c r="AG3" s="5"/>
-      <c r="AH3" s="6"/>
-      <c r="AI3" s="6"/>
+    <row r="3" spans="1:34" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A3" s="7"/>
+      <c r="B3" s="7"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="10"/>
+      <c r="K3" s="11"/>
+      <c r="L3" s="9"/>
+      <c r="M3" s="12"/>
+      <c r="N3" s="9"/>
+      <c r="O3" s="12"/>
+      <c r="P3" s="9"/>
+      <c r="Q3" s="12"/>
+      <c r="R3" s="9"/>
+      <c r="S3" s="12"/>
+      <c r="T3" s="9"/>
+      <c r="U3" s="12"/>
+      <c r="V3" s="9"/>
+      <c r="W3" s="12"/>
+      <c r="X3" s="9"/>
+      <c r="Y3" s="12"/>
+      <c r="Z3" s="9"/>
+      <c r="AA3" s="12"/>
+      <c r="AB3" s="9"/>
+      <c r="AC3" s="12"/>
+      <c r="AD3" s="9"/>
+      <c r="AE3" s="12"/>
+      <c r="AF3" s="9"/>
+      <c r="AG3" s="12"/>
+      <c r="AH3" s="9"/>
     </row>
-    <row r="4" spans="1:35" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="13"/>
-      <c r="B4" s="13"/>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
-      <c r="G4" s="13"/>
-      <c r="H4" s="13"/>
-      <c r="I4" s="13"/>
-      <c r="J4" s="9"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="6"/>
-      <c r="M4" s="5"/>
-      <c r="N4" s="6"/>
-      <c r="O4" s="5"/>
-      <c r="P4" s="6"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="6"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="6"/>
-      <c r="U4" s="5"/>
-      <c r="V4" s="6"/>
-      <c r="W4" s="5"/>
-      <c r="X4" s="6"/>
-      <c r="Y4" s="5"/>
-      <c r="Z4" s="6"/>
-      <c r="AA4" s="5"/>
-      <c r="AB4" s="6"/>
-      <c r="AC4" s="5"/>
-      <c r="AD4" s="6"/>
-      <c r="AE4" s="5"/>
-      <c r="AF4" s="6"/>
-      <c r="AG4" s="5"/>
-      <c r="AH4" s="6"/>
-      <c r="AI4" s="6"/>
+    <row r="4" spans="1:34" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="7"/>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+      <c r="G4" s="7"/>
+      <c r="H4" s="7"/>
+      <c r="I4" s="7"/>
+      <c r="J4" s="10"/>
+      <c r="K4" s="11"/>
+      <c r="L4" s="9"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="9"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="9"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="9"/>
+      <c r="S4" s="12"/>
+      <c r="T4" s="9"/>
+      <c r="U4" s="12"/>
+      <c r="V4" s="9"/>
+      <c r="W4" s="12"/>
+      <c r="X4" s="9"/>
+      <c r="Y4" s="12"/>
+      <c r="Z4" s="9"/>
+      <c r="AA4" s="12"/>
+      <c r="AB4" s="9"/>
+      <c r="AC4" s="12"/>
+      <c r="AD4" s="9"/>
+      <c r="AE4" s="12"/>
+      <c r="AF4" s="9"/>
+      <c r="AG4" s="12"/>
+      <c r="AH4" s="9"/>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
+    <row r="5" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A5" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="C5" s="14"/>
-      <c r="D5" s="14"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="14"/>
-      <c r="G5" s="14"/>
-      <c r="H5" s="14"/>
-      <c r="I5" s="14"/>
-      <c r="J5" s="9"/>
-      <c r="K5" s="10"/>
-      <c r="L5" s="6"/>
-      <c r="M5" s="5"/>
-      <c r="N5" s="6"/>
-      <c r="O5" s="5"/>
-      <c r="P5" s="6"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="6"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="6"/>
-      <c r="U5" s="5"/>
-      <c r="V5" s="6"/>
-      <c r="W5" s="5"/>
-      <c r="X5" s="6"/>
-      <c r="Y5" s="5"/>
-      <c r="Z5" s="6"/>
-      <c r="AA5" s="5"/>
-      <c r="AB5" s="6"/>
-      <c r="AC5" s="5"/>
-      <c r="AD5" s="6"/>
-      <c r="AE5" s="5"/>
-      <c r="AF5" s="6"/>
-      <c r="AG5" s="5"/>
-      <c r="AH5" s="6"/>
-      <c r="AI5" s="6"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="8"/>
+      <c r="I5" s="8"/>
+      <c r="J5" s="10"/>
+      <c r="K5" s="11"/>
+      <c r="L5" s="9"/>
+      <c r="M5" s="12"/>
+      <c r="N5" s="9"/>
+      <c r="O5" s="12"/>
+      <c r="P5" s="9"/>
+      <c r="Q5" s="12"/>
+      <c r="R5" s="9"/>
+      <c r="S5" s="12"/>
+      <c r="T5" s="9"/>
+      <c r="U5" s="12"/>
+      <c r="V5" s="9"/>
+      <c r="W5" s="12"/>
+      <c r="X5" s="9"/>
+      <c r="Y5" s="12"/>
+      <c r="Z5" s="9"/>
+      <c r="AA5" s="12"/>
+      <c r="AB5" s="9"/>
+      <c r="AC5" s="12"/>
+      <c r="AD5" s="9"/>
+      <c r="AE5" s="12"/>
+      <c r="AF5" s="9"/>
+      <c r="AG5" s="12"/>
+      <c r="AH5" s="9"/>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A6" s="14"/>
-      <c r="B6" s="14"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="14"/>
-      <c r="G6" s="14"/>
-      <c r="H6" s="14"/>
-      <c r="I6" s="14"/>
-      <c r="J6" s="9"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="5"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="5"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="5"/>
-      <c r="R6" s="6"/>
-      <c r="S6" s="5"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="5"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="5"/>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="5"/>
-      <c r="Z6" s="6"/>
-      <c r="AA6" s="5"/>
-      <c r="AB6" s="6"/>
-      <c r="AC6" s="5"/>
-      <c r="AD6" s="6"/>
-      <c r="AE6" s="5"/>
-      <c r="AF6" s="6"/>
-      <c r="AG6" s="5"/>
-      <c r="AH6" s="6"/>
-      <c r="AI6" s="6"/>
+    <row r="6" spans="1:34" x14ac:dyDescent="0.25">
+      <c r="A6" s="8"/>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+      <c r="G6" s="8"/>
+      <c r="H6" s="8"/>
+      <c r="I6" s="8"/>
+      <c r="J6" s="10"/>
+      <c r="K6" s="11"/>
+      <c r="L6" s="9"/>
+      <c r="M6" s="12"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="12"/>
+      <c r="P6" s="9"/>
+      <c r="Q6" s="12"/>
+      <c r="R6" s="9"/>
+      <c r="S6" s="12"/>
+      <c r="T6" s="9"/>
+      <c r="U6" s="12"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="12"/>
+      <c r="X6" s="9"/>
+      <c r="Y6" s="12"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="12"/>
+      <c r="AB6" s="9"/>
+      <c r="AC6" s="12"/>
+      <c r="AD6" s="9"/>
+      <c r="AE6" s="12"/>
+      <c r="AF6" s="9"/>
+      <c r="AG6" s="12"/>
+      <c r="AH6" s="9"/>
     </row>
-    <row r="7" spans="1:35" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:34" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C7" s="11"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="11"/>
-      <c r="I7" s="11"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
       <c r="J7" s="3"/>
       <c r="K7" s="4"/>
       <c r="L7" s="3"/>
@@ -1076,26 +1065,23 @@
       <c r="AF7" s="3"/>
       <c r="AG7" s="4"/>
       <c r="AH7" s="3"/>
-      <c r="AI7" s="3" t="s">
-        <v>44</v>
-      </c>
     </row>
-    <row r="8" spans="1:35" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:34" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="11"/>
-      <c r="D8" s="11"/>
-      <c r="E8" s="11"/>
-      <c r="F8" s="11"/>
-      <c r="G8" s="11"/>
-      <c r="H8" s="11"/>
-      <c r="I8" s="11"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
       <c r="J8" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K8" s="4"/>
       <c r="L8" s="3"/>
@@ -1121,25 +1107,24 @@
       <c r="AF8" s="3"/>
       <c r="AG8" s="4"/>
       <c r="AH8" s="3"/>
-      <c r="AI8" s="3"/>
     </row>
-    <row r="9" spans="1:35" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:34" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="11"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="11"/>
-      <c r="I9" s="11"/>
+      <c r="C9" s="5"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
       <c r="J9" s="3"/>
       <c r="K9" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L9" s="3"/>
       <c r="M9" s="4"/>
@@ -1164,22 +1149,21 @@
       <c r="AF9" s="3"/>
       <c r="AG9" s="4"/>
       <c r="AH9" s="3"/>
-      <c r="AI9" s="3"/>
     </row>
-    <row r="10" spans="1:35" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:34" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="11"/>
-      <c r="G10" s="11"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="11"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
       <c r="J10" s="3"/>
       <c r="K10" s="4"/>
       <c r="L10" s="3"/>
@@ -1193,7 +1177,7 @@
       <c r="T10" s="3"/>
       <c r="U10" s="4"/>
       <c r="V10" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="W10" s="4"/>
       <c r="X10" s="3"/>
@@ -1207,24 +1191,23 @@
       <c r="AF10" s="3"/>
       <c r="AG10" s="4"/>
       <c r="AH10" s="3"/>
-      <c r="AI10" s="3"/>
     </row>
-    <row r="11" spans="1:35" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:34" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C11" s="11"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="11"/>
+      <c r="C11" s="5"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
       <c r="J11" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K11" s="4"/>
       <c r="L11" s="3"/>
@@ -1250,24 +1233,23 @@
       <c r="AF11" s="3"/>
       <c r="AG11" s="4"/>
       <c r="AH11" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI11" s="3"/>
+        <v>42</v>
+      </c>
     </row>
-    <row r="12" spans="1:35" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:34" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B12" s="11" t="s">
+      <c r="B12" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C12" s="11"/>
-      <c r="D12" s="11"/>
-      <c r="E12" s="11"/>
-      <c r="F12" s="11"/>
-      <c r="G12" s="11"/>
-      <c r="H12" s="11"/>
-      <c r="I12" s="11"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
       <c r="J12" s="3"/>
       <c r="K12" s="4"/>
       <c r="L12" s="3"/>
@@ -1293,24 +1275,23 @@
       <c r="AF12" s="3"/>
       <c r="AG12" s="4"/>
       <c r="AH12" s="3"/>
-      <c r="AI12" s="3"/>
     </row>
-    <row r="13" spans="1:35" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:34" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B13" s="11" t="s">
+      <c r="B13" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="11"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="11"/>
-      <c r="I13" s="11"/>
+      <c r="C13" s="5"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
       <c r="J13" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K13" s="4"/>
       <c r="L13" s="3"/>
@@ -1336,24 +1317,23 @@
       <c r="AF13" s="3"/>
       <c r="AG13" s="4"/>
       <c r="AH13" s="3"/>
-      <c r="AI13" s="3"/>
     </row>
-    <row r="14" spans="1:35" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:34" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B14" s="12" t="s">
+      <c r="B14" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12"/>
-      <c r="E14" s="12"/>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="12"/>
-      <c r="I14" s="12"/>
+      <c r="C14" s="6"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
       <c r="J14" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K14" s="4"/>
       <c r="L14" s="3"/>
@@ -1379,27 +1359,26 @@
       <c r="AF14" s="3"/>
       <c r="AG14" s="4"/>
       <c r="AH14" s="3"/>
-      <c r="AI14" s="3"/>
     </row>
-    <row r="15" spans="1:35" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:34" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B15" s="12" t="s">
-        <v>46</v>
-      </c>
-      <c r="C15" s="12"/>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
-      <c r="G15" s="12"/>
-      <c r="H15" s="12"/>
-      <c r="I15" s="12"/>
+        <v>44</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="6"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
+      <c r="G15" s="6"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
       <c r="J15" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="K15" s="4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="L15" s="3"/>
       <c r="M15" s="4"/>
@@ -1412,7 +1391,7 @@
       <c r="T15" s="3"/>
       <c r="U15" s="4"/>
       <c r="V15" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="W15" s="4"/>
       <c r="X15" s="3"/>
@@ -1426,12 +1405,37 @@
       <c r="AF15" s="3"/>
       <c r="AG15" s="4"/>
       <c r="AH15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="AI15" s="3"/>
+        <v>42</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="39">
+  <mergeCells count="38">
+    <mergeCell ref="AG2:AG6"/>
+    <mergeCell ref="AH2:AH6"/>
+    <mergeCell ref="J1:AH1"/>
+    <mergeCell ref="AA2:AA6"/>
+    <mergeCell ref="AB2:AB6"/>
+    <mergeCell ref="AC2:AC6"/>
+    <mergeCell ref="AD2:AD6"/>
+    <mergeCell ref="AE2:AE6"/>
+    <mergeCell ref="AF2:AF6"/>
+    <mergeCell ref="U2:U6"/>
+    <mergeCell ref="V2:V6"/>
+    <mergeCell ref="W2:W6"/>
+    <mergeCell ref="X2:X6"/>
+    <mergeCell ref="Y2:Y6"/>
+    <mergeCell ref="Z2:Z6"/>
+    <mergeCell ref="T2:T6"/>
+    <mergeCell ref="J2:J6"/>
+    <mergeCell ref="K2:K6"/>
+    <mergeCell ref="L2:L6"/>
+    <mergeCell ref="M2:M6"/>
+    <mergeCell ref="N2:N6"/>
+    <mergeCell ref="O2:O6"/>
+    <mergeCell ref="P2:P6"/>
+    <mergeCell ref="Q2:Q6"/>
+    <mergeCell ref="R2:R6"/>
+    <mergeCell ref="S2:S6"/>
     <mergeCell ref="B9:I9"/>
     <mergeCell ref="B15:I15"/>
     <mergeCell ref="A1:I4"/>
@@ -1444,33 +1448,6 @@
     <mergeCell ref="B12:I12"/>
     <mergeCell ref="B13:I13"/>
     <mergeCell ref="B14:I14"/>
-    <mergeCell ref="T2:T6"/>
-    <mergeCell ref="J2:J6"/>
-    <mergeCell ref="K2:K6"/>
-    <mergeCell ref="L2:L6"/>
-    <mergeCell ref="M2:M6"/>
-    <mergeCell ref="N2:N6"/>
-    <mergeCell ref="O2:O6"/>
-    <mergeCell ref="P2:P6"/>
-    <mergeCell ref="Q2:Q6"/>
-    <mergeCell ref="R2:R6"/>
-    <mergeCell ref="S2:S6"/>
-    <mergeCell ref="AG2:AG6"/>
-    <mergeCell ref="AH2:AH6"/>
-    <mergeCell ref="AI2:AI6"/>
-    <mergeCell ref="J1:AI1"/>
-    <mergeCell ref="AA2:AA6"/>
-    <mergeCell ref="AB2:AB6"/>
-    <mergeCell ref="AC2:AC6"/>
-    <mergeCell ref="AD2:AD6"/>
-    <mergeCell ref="AE2:AE6"/>
-    <mergeCell ref="AF2:AF6"/>
-    <mergeCell ref="U2:U6"/>
-    <mergeCell ref="V2:V6"/>
-    <mergeCell ref="W2:W6"/>
-    <mergeCell ref="X2:X6"/>
-    <mergeCell ref="Y2:Y6"/>
-    <mergeCell ref="Z2:Z6"/>
   </mergeCells>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>